<commit_message>
Update Balance sheet (Simple).xlsx
STEP 6
</commit_message>
<xml_diff>
--- a/Finance/Balance sheet (Simple).xlsx
+++ b/Finance/Balance sheet (Simple).xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\i074178\Documents\GitHub\Document\Finance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DCE8E37-E85F-4D9A-97D5-4BCA3454375A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D348B20-0034-4715-8B4F-2D9C18CB173E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45972" yWindow="-1440" windowWidth="14616" windowHeight="22656" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="45972" yWindow="-1440" windowWidth="14616" windowHeight="22656" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Start" sheetId="5" r:id="rId1"/>
     <sheet name="Balance sheet" sheetId="2" r:id="rId2"/>
-    <sheet name="Year-over-year chart" sheetId="3" r:id="rId3"/>
-    <sheet name="Financial Activity" sheetId="6" r:id="rId4"/>
-    <sheet name="Account Balance" sheetId="7" r:id="rId5"/>
+    <sheet name="Financial Activity" sheetId="6" r:id="rId3"/>
+    <sheet name="Account Balance" sheetId="7" r:id="rId4"/>
+    <sheet name="Year-over-year chart" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <webPublishing codePage="1252"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="69">
   <si>
     <t>Assets</t>
   </si>
@@ -225,6 +225,21 @@
   </si>
   <si>
     <t>Short-term borrowing</t>
+  </si>
+  <si>
+    <t>3. 购买生产设备，花费5700万</t>
+  </si>
+  <si>
+    <t>4. 获取一块土地使用权，花费150万</t>
+  </si>
+  <si>
+    <t>Intangible assets</t>
+  </si>
+  <si>
+    <t>5. 采购原材料花费2400万，支付了1600万，剩余将在下一年度支付</t>
+  </si>
+  <si>
+    <t>6. 生产出一批产品，产品成本3600万，其中原材料2400万，人工费和其他支出1200万，以现金支付</t>
   </si>
 </sst>
 </file>
@@ -444,7 +459,7 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -531,6 +546,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="43" fontId="8" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="4" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -543,11 +564,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="4" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="43" fontId="9" fillId="6" borderId="0" xfId="3" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -558,6 +576,11 @@
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="55">
+    <dxf>
+      <font>
+        <color indexed="10"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -579,7 +602,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor theme="0"/>
-          <bgColor theme="5" tint="0.39997558519241921"/>
+          <bgColor theme="4" tint="0.39997558519241921"/>
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -612,7 +635,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor theme="0"/>
-          <bgColor theme="5" tint="0.39997558519241921"/>
+          <bgColor theme="4" tint="0.39997558519241921"/>
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -644,7 +667,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor theme="0"/>
-          <bgColor theme="5" tint="0.39997558519241921"/>
+          <bgColor theme="4" tint="0.39997558519241921"/>
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -678,7 +701,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor theme="0"/>
-          <bgColor theme="5" tint="0.39997558519241921"/>
+          <bgColor theme="4" tint="0.39997558519241921"/>
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -711,7 +734,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor theme="0"/>
-          <bgColor theme="5" tint="0.39997558519241921"/>
+          <bgColor theme="4" tint="0.39997558519241921"/>
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -743,7 +766,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor theme="0"/>
-          <bgColor theme="5" tint="0.39997558519241921"/>
+          <bgColor theme="4" tint="0.39997558519241921"/>
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -790,6 +813,12 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid"/>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -823,6 +852,12 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid"/>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -856,23 +891,6 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <color indexed="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid"/>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid"/>
       </fill>
@@ -896,67 +914,6 @@
         <patternFill patternType="solid">
           <fgColor theme="0"/>
           <bgColor theme="4" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid"/>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="0"/>
-          <bgColor theme="5" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="0"/>
-          <bgColor theme="5" tint="0.39997558519241921"/>
         </patternFill>
       </fill>
     </dxf>
@@ -984,7 +941,7 @@
           <bgColor theme="5" tint="0.39997558519241921"/>
         </patternFill>
       </fill>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
         <top/>
@@ -1023,7 +980,7 @@
           <bgColor theme="5" tint="0.39997558519241921"/>
         </patternFill>
       </fill>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
         <top/>
@@ -1062,7 +1019,7 @@
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
         <top/>
@@ -1070,67 +1027,6 @@
           <color indexed="64"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid"/>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="0"/>
-          <bgColor theme="5" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="0"/>
-          <bgColor theme="5" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid"/>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="solid"/>
-      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -1202,7 +1098,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor theme="0"/>
-          <bgColor theme="4" tint="0.39997558519241921"/>
+          <bgColor theme="5" tint="0.39997558519241921"/>
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0">
@@ -1241,7 +1137,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor theme="0"/>
-          <bgColor theme="4" tint="0.39997558519241921"/>
+          <bgColor theme="5" tint="0.39997558519241921"/>
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0">
@@ -1279,7 +1175,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor theme="0"/>
-          <bgColor theme="4" tint="0.39997558519241921"/>
+          <bgColor theme="5" tint="0.39997558519241921"/>
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1299,10 +1195,21 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
       <fill>
         <patternFill patternType="solid">
           <fgColor theme="0"/>
-          <bgColor theme="4" tint="0.39997558519241921"/>
+          <bgColor theme="5" tint="0.39997558519241921"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1312,10 +1219,21 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
       <fill>
         <patternFill patternType="solid">
           <fgColor theme="0"/>
-          <bgColor theme="4" tint="0.39997558519241921"/>
+          <bgColor theme="5" tint="0.39997558519241921"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1340,10 +1258,10 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor theme="0"/>
-          <bgColor theme="4" tint="0.39997558519241921"/>
+          <bgColor theme="5" tint="0.39997558519241921"/>
         </patternFill>
       </fill>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
         <top/>
@@ -1379,10 +1297,10 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor theme="0"/>
-          <bgColor theme="4" tint="0.39997558519241921"/>
+          <bgColor theme="5" tint="0.39997558519241921"/>
         </patternFill>
       </fill>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
         <top/>
@@ -1417,11 +1335,11 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor theme="0"/>
-          <bgColor theme="4" tint="0.39997558519241921"/>
+          <bgColor theme="5" tint="0.39997558519241921"/>
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
         <top/>
@@ -1429,6 +1347,106 @@
           <color indexed="64"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid"/>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0"/>
+          <bgColor theme="5" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0"/>
+          <bgColor theme="5" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid"/>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0"/>
+          <bgColor theme="4" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0"/>
+          <bgColor theme="4" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid"/>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="solid"/>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -1547,9 +1565,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>('Balance sheet'!$B$6:$B$12,'Balance sheet'!$B$15:$B$19,'Balance sheet'!$B$22:$B$23,'Balance sheet'!$B$29:$B$36,'Balance sheet'!$B$39:$B$40,'Balance sheet'!$B$43:$B$45)</c:f>
+              <c:f>('Balance sheet'!$B$6:$B$12,'Balance sheet'!$B$15:$B$19,'Balance sheet'!$B$22:$B$24,'Balance sheet'!$B$30:$B$37,'Balance sheet'!$B$40:$B$41,'Balance sheet'!$B$44:$B$46)</c:f>
               <c:strCache>
-                <c:ptCount val="27"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
                   <c:v>Cash</c:v>
                 </c:pt>
@@ -1587,48 +1605,51 @@
                   <c:v>Total fixed assets</c:v>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v>Intangible assets</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>Goodwill</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>Total other assets</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>Accounts payable</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>Accrued wages</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>Accrued compensation</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>Income taxes payable</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>Unearned revenue</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>Short-term borrowing</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>Other</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="22">
                   <c:v>Total current liabilities</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
                   <c:v>Mortgage payable</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
                   <c:v>Total long-term liabilities</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>Capital stock</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
                   <c:v>Accumulated retained earnings</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="27">
                   <c:v>Total owner's equity</c:v>
                 </c:pt>
               </c:strCache>
@@ -1636,89 +1657,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>('Balance sheet'!$C$6:$C$12,'Balance sheet'!$C$15:$C$19,'Balance sheet'!$C$22:$C$23,'Balance sheet'!$C$29:$C$36,'Balance sheet'!$C$39:$C$40,'Balance sheet'!$C$43:$C$45)</c:f>
-              <c:numCache>
-                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="27"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
+              <c:f>('Balance sheet'!$C$6:$C$12,'Balance sheet'!$C$15:$C$19,'Balance sheet'!$C$22:$C$24,'Balance sheet'!$C$30:$C$37,'Balance sheet'!$C$40:$C$41,'Balance sheet'!$C$44:$C$46)</c:f>
             </c:numRef>
           </c:val>
           <c:extLst>
@@ -1741,9 +1680,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>('Balance sheet'!$B$6:$B$12,'Balance sheet'!$B$15:$B$19,'Balance sheet'!$B$22:$B$23,'Balance sheet'!$B$29:$B$36,'Balance sheet'!$B$39:$B$40,'Balance sheet'!$B$43:$B$45)</c:f>
+              <c:f>('Balance sheet'!$B$6:$B$12,'Balance sheet'!$B$15:$B$19,'Balance sheet'!$B$22:$B$24,'Balance sheet'!$B$30:$B$37,'Balance sheet'!$B$40:$B$41,'Balance sheet'!$B$44:$B$46)</c:f>
               <c:strCache>
-                <c:ptCount val="27"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
                   <c:v>Cash</c:v>
                 </c:pt>
@@ -1781,48 +1720,51 @@
                   <c:v>Total fixed assets</c:v>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v>Intangible assets</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>Goodwill</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>Total other assets</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>Accounts payable</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>Accrued wages</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>Accrued compensation</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>Income taxes payable</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>Unearned revenue</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>Short-term borrowing</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>Other</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="22">
                   <c:v>Total current liabilities</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
                   <c:v>Mortgage payable</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
                   <c:v>Total long-term liabilities</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>Capital stock</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
                   <c:v>Accumulated retained earnings</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="27">
                   <c:v>Total owner's equity</c:v>
                 </c:pt>
               </c:strCache>
@@ -1830,18 +1772,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>('Balance sheet'!$D$6:$D$12,'Balance sheet'!$D$15:$D$19,'Balance sheet'!$D$22:$D$23,'Balance sheet'!$D$29:$D$36,'Balance sheet'!$D$39:$D$40,'Balance sheet'!$D$43:$D$45)</c:f>
+              <c:f>('Balance sheet'!$D$6:$D$12,'Balance sheet'!$D$15:$D$19,'Balance sheet'!$D$22:$D$24,'Balance sheet'!$D$30:$D$37,'Balance sheet'!$D$40:$D$41,'Balance sheet'!$D$44:$D$46)</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
-                  <c:v>8300</c:v>
+                  <c:v>-350</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>3600</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -1853,10 +1795,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8300</c:v>
+                  <c:v>3250</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>5700</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -1868,19 +1810,19 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>5700</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>800</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>0</c:v>
@@ -1892,27 +1834,30 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>5100</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="21">
-                  <c:v>5100</c:v>
-                </c:pt>
                 <c:pt idx="22">
-                  <c:v>0</c:v>
+                  <c:v>5900</c:v>
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="24">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>3200</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="26">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="27">
                   <c:v>3200</c:v>
                 </c:pt>
               </c:numCache>
@@ -2048,9 +1993,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="FixedAssets" displayName="FixedAssets" ref="B14:D19" totalsRowCount="1" headerRowDxfId="54" dataDxfId="53" totalsRowDxfId="52" dataCellStyle="Emphasis 1">
   <autoFilter ref="B14:D18" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Fixed assets:" totalsRowLabel="Total fixed assets" dataDxfId="51" totalsRowDxfId="50" dataCellStyle="Emphasis 1"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Previous Year" totalsRowFunction="sum" dataDxfId="49" totalsRowDxfId="48" dataCellStyle="Emphasis 1"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Current Year" totalsRowFunction="sum" dataDxfId="47" totalsRowDxfId="46" dataCellStyle="Emphasis 1"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Fixed assets:" totalsRowLabel="Total fixed assets" dataDxfId="51" totalsRowDxfId="6" dataCellStyle="Emphasis 1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Previous Year" totalsRowFunction="sum" dataDxfId="50" totalsRowDxfId="5" dataCellStyle="Emphasis 1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Current Year" totalsRowFunction="sum" dataDxfId="49" totalsRowDxfId="4" dataCellStyle="Emphasis 1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -2062,12 +2007,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="OtherAssets" displayName="OtherAssets" ref="B21:D23" totalsRowCount="1" headerRowDxfId="45" dataDxfId="44" totalsRowDxfId="43" dataCellStyle="Emphasis 1">
-  <autoFilter ref="B21:D22" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="OtherAssets" displayName="OtherAssets" ref="B21:D24" totalsRowCount="1" headerRowDxfId="48" dataDxfId="47" totalsRowDxfId="46" dataCellStyle="Emphasis 1">
+  <autoFilter ref="B21:D23" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Other assets:" totalsRowLabel="Total other assets" dataDxfId="42" totalsRowDxfId="41" dataCellStyle="Emphasis 1"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Previous Year" totalsRowFunction="sum" dataDxfId="40" totalsRowDxfId="39" dataCellStyle="Emphasis 1"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Current Year" totalsRowFunction="sum" dataDxfId="38" totalsRowDxfId="37" dataCellStyle="Emphasis 1"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Other assets:" totalsRowLabel="Total other assets" dataDxfId="45" totalsRowDxfId="3" dataCellStyle="Emphasis 1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Previous Year" totalsRowFunction="sum" dataDxfId="44" totalsRowDxfId="2" dataCellStyle="Emphasis 1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Current Year" totalsRowFunction="sum" dataDxfId="43" totalsRowDxfId="1" dataCellStyle="Emphasis 1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -2079,12 +2024,12 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="CurrentLiabilities" displayName="CurrentLiabilities" ref="B28:D36" totalsRowCount="1" headerRowDxfId="36" dataDxfId="35" totalsRowDxfId="34" headerRowCellStyle="Emphasis 2" dataCellStyle="Emphasis 2" totalsRowCellStyle="Emphasis 2">
-  <autoFilter ref="B28:D35" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="CurrentLiabilities" displayName="CurrentLiabilities" ref="B29:D37" totalsRowCount="1" headerRowDxfId="42" dataDxfId="41" totalsRowDxfId="40" headerRowCellStyle="Emphasis 2" dataCellStyle="Emphasis 2" totalsRowCellStyle="Emphasis 2">
+  <autoFilter ref="B29:D36" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Current liabilities:" totalsRowLabel="Total current liabilities" dataDxfId="33" totalsRowDxfId="5" dataCellStyle="Emphasis 2"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Previous Year" totalsRowFunction="sum" dataDxfId="32" totalsRowDxfId="4" dataCellStyle="Emphasis 2"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Current Year" totalsRowFunction="sum" dataDxfId="31" totalsRowDxfId="3" dataCellStyle="Emphasis 2"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Current liabilities:" totalsRowLabel="Total current liabilities" dataDxfId="39" totalsRowDxfId="38" dataCellStyle="Emphasis 2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Previous Year" totalsRowFunction="sum" dataDxfId="37" totalsRowDxfId="36" dataCellStyle="Emphasis 2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Current Year" totalsRowFunction="sum" dataDxfId="35" totalsRowDxfId="34" dataCellStyle="Emphasis 2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -2096,12 +2041,12 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="LongTermLiabilities" displayName="LongTermLiabilities" ref="B38:D40" totalsRowCount="1" headerRowDxfId="30" dataDxfId="29" totalsRowDxfId="28" headerRowCellStyle="Emphasis 2" dataCellStyle="Emphasis 2" totalsRowCellStyle="Emphasis 2">
-  <autoFilter ref="B38:D39" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="LongTermLiabilities" displayName="LongTermLiabilities" ref="B39:D41" totalsRowCount="1" headerRowDxfId="33" dataDxfId="32" totalsRowDxfId="31" headerRowCellStyle="Emphasis 2" dataCellStyle="Emphasis 2" totalsRowCellStyle="Emphasis 2">
+  <autoFilter ref="B39:D40" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Long-term liabilities:" totalsRowLabel="Total long-term liabilities" dataDxfId="27" totalsRowDxfId="26" dataCellStyle="Emphasis 2"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Previous Year" totalsRowFunction="sum" dataDxfId="25" totalsRowDxfId="24" dataCellStyle="Emphasis 2"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Current Year" totalsRowFunction="sum" dataDxfId="23" totalsRowDxfId="22" dataCellStyle="Emphasis 2"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Long-term liabilities:" totalsRowLabel="Total long-term liabilities" dataDxfId="30" totalsRowDxfId="29" dataCellStyle="Emphasis 2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Previous Year" totalsRowFunction="sum" dataDxfId="28" totalsRowDxfId="27" dataCellStyle="Emphasis 2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Current Year" totalsRowFunction="sum" dataDxfId="26" totalsRowDxfId="25" dataCellStyle="Emphasis 2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -2113,13 +2058,13 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="OwnersEquity" displayName="OwnersEquity" ref="B42:D45" totalsRowCount="1" headerRowDxfId="21" dataDxfId="20" totalsRowDxfId="19" headerRowCellStyle="Emphasis 2" dataCellStyle="Emphasis 2" totalsRowCellStyle="Emphasis 2">
-  <autoFilter ref="B42:D44" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="OwnersEquity" displayName="OwnersEquity" ref="B43:D46" totalsRowCount="1" headerRowDxfId="24" dataDxfId="23" totalsRowDxfId="22" headerRowCellStyle="Emphasis 2" dataCellStyle="Emphasis 2" totalsRowCellStyle="Emphasis 2">
+  <autoFilter ref="B43:D45" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Owner's equity:" totalsRowLabel="Total owner's equity" dataDxfId="18" totalsRowDxfId="2" dataCellStyle="Emphasis 2"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Previous Year" totalsRowFunction="sum" dataDxfId="17" totalsRowDxfId="1" dataCellStyle="Emphasis 2"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Current Year" totalsRowFunction="sum" dataDxfId="16" totalsRowDxfId="0" dataCellStyle="Emphasis 2">
-      <calculatedColumnFormula>SUMIF('Account Balance'!A:A,OwnersEquity[[#This Row],[Owner''s equity:]],'Account Balance'!B:B)</calculatedColumnFormula>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Owner's equity:" totalsRowLabel="Total owner's equity" dataDxfId="21" totalsRowDxfId="20" dataCellStyle="Emphasis 2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Previous Year" totalsRowFunction="sum" dataDxfId="19" totalsRowDxfId="18" dataCellStyle="Emphasis 2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Current Year" totalsRowFunction="sum" dataDxfId="17" totalsRowDxfId="16" dataCellStyle="Emphasis 2">
+      <calculatedColumnFormula>SUMIF('Account Balance'!B:B,OwnersEquity[[#This Row],[Owner''s equity:]],'Account Balance'!C:C)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2135,10 +2080,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="CurrentAssets" displayName="CurrentAssets" ref="B5:D12" totalsRowCount="1" headerRowDxfId="15" dataDxfId="14" totalsRowDxfId="13" dataCellStyle="Emphasis 1">
   <autoFilter ref="B5:D11" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Current assets:" totalsRowLabel="Total current assets" dataDxfId="12" totalsRowDxfId="8" dataCellStyle="Emphasis 1" totalsRowCellStyle="Emphasis 1"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Previous Year" totalsRowFunction="sum" dataDxfId="11" totalsRowDxfId="7" dataCellStyle="Emphasis 1" totalsRowCellStyle="Emphasis 1"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Current Year" totalsRowFunction="sum" dataDxfId="10" totalsRowDxfId="6" dataCellStyle="Emphasis 1" totalsRowCellStyle="Emphasis 1">
-      <calculatedColumnFormula>SUMIF('Account Balance'!A:A,CurrentAssets[[#This Row],[Current assets:]],'Account Balance'!B:B)</calculatedColumnFormula>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Current assets:" totalsRowLabel="Total current assets" dataDxfId="12" totalsRowDxfId="11" dataCellStyle="Emphasis 1" totalsRowCellStyle="Emphasis 1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Previous Year" totalsRowFunction="sum" dataDxfId="10" totalsRowDxfId="9" dataCellStyle="Emphasis 1" totalsRowCellStyle="Emphasis 1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Current Year" totalsRowFunction="sum" dataDxfId="8" totalsRowDxfId="7" dataCellStyle="Emphasis 1" totalsRowCellStyle="Emphasis 1">
+      <calculatedColumnFormula>SUMIF('Account Balance'!B:B,CurrentAssets[[#This Row],[Current assets:]],'Account Balance'!C:C)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2539,17 +2484,17 @@
     <tabColor theme="4" tint="-0.249977111117893"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D50"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+    <sheetView showGridLines="0" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2.6640625" style="18" customWidth="1"/>
     <col min="2" max="2" width="46.6640625" style="13" customWidth="1"/>
-    <col min="3" max="3" width="5.21875" style="13" customWidth="1"/>
+    <col min="3" max="3" width="5.21875" style="13" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="17.5546875" style="13" customWidth="1"/>
     <col min="5" max="5" width="2.6640625" customWidth="1"/>
   </cols>
@@ -2558,11 +2503,11 @@
       <c r="A1" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="44"/>
-      <c r="D1" s="46" t="s">
+      <c r="C1" s="46"/>
+      <c r="D1" s="48" t="s">
         <v>30</v>
       </c>
     </row>
@@ -2570,9 +2515,9 @@
       <c r="A2" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="47"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="49"/>
     </row>
     <row r="3" spans="1:4" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="1"/>
@@ -2611,8 +2556,8 @@
         <v>0</v>
       </c>
       <c r="D6" s="24">
-        <f>SUMIF('Account Balance'!A:A,CurrentAssets[[#This Row],[Current assets:]],'Account Balance'!B:B)</f>
-        <v>8300</v>
+        <f>SUMIF('Account Balance'!B:B,CurrentAssets[[#This Row],[Current assets:]],'Account Balance'!C:C)</f>
+        <v>-350</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -2623,7 +2568,7 @@
         <v>0</v>
       </c>
       <c r="D7" s="24">
-        <f>SUMIF('Account Balance'!A:A,CurrentAssets[[#This Row],[Current assets:]],'Account Balance'!B:B)</f>
+        <f>SUMIF('Account Balance'!B:B,CurrentAssets[[#This Row],[Current assets:]],'Account Balance'!C:C)</f>
         <v>0</v>
       </c>
     </row>
@@ -2635,8 +2580,8 @@
         <v>0</v>
       </c>
       <c r="D8" s="24">
-        <f>SUMIF('Account Balance'!A:A,CurrentAssets[[#This Row],[Current assets:]],'Account Balance'!B:B)</f>
-        <v>0</v>
+        <f>SUMIF('Account Balance'!B:B,CurrentAssets[[#This Row],[Current assets:]],'Account Balance'!C:C)</f>
+        <v>3600</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -2647,7 +2592,7 @@
         <v>0</v>
       </c>
       <c r="D9" s="24">
-        <f>SUMIF('Account Balance'!A:A,CurrentAssets[[#This Row],[Current assets:]],'Account Balance'!B:B)</f>
+        <f>SUMIF('Account Balance'!B:B,CurrentAssets[[#This Row],[Current assets:]],'Account Balance'!C:C)</f>
         <v>0</v>
       </c>
     </row>
@@ -2659,7 +2604,7 @@
         <v>0</v>
       </c>
       <c r="D10" s="24">
-        <f>SUMIF('Account Balance'!A:A,CurrentAssets[[#This Row],[Current assets:]],'Account Balance'!B:B)</f>
+        <f>SUMIF('Account Balance'!B:B,CurrentAssets[[#This Row],[Current assets:]],'Account Balance'!C:C)</f>
         <v>0</v>
       </c>
     </row>
@@ -2671,7 +2616,7 @@
         <v>0</v>
       </c>
       <c r="D11" s="24">
-        <f>SUMIF('Account Balance'!A:A,CurrentAssets[[#This Row],[Current assets:]],'Account Balance'!B:B)</f>
+        <f>SUMIF('Account Balance'!B:B,CurrentAssets[[#This Row],[Current assets:]],'Account Balance'!C:C)</f>
         <v>0</v>
       </c>
     </row>
@@ -2685,7 +2630,7 @@
       </c>
       <c r="D12" s="27">
         <f>SUBTOTAL(109,CurrentAssets[Current Year])</f>
-        <v>8300</v>
+        <v>3250</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -2715,7 +2660,8 @@
         <v>0</v>
       </c>
       <c r="D15" s="24">
-        <v>0</v>
+        <f>SUMIF('Account Balance'!B:B,FixedAssets[[#This Row],[Fixed assets:]],'Account Balance'!C:C)</f>
+        <v>5700</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -2761,7 +2707,7 @@
       </c>
       <c r="D19" s="27">
         <f>SUBTOTAL(109,FixedAssets[Current Year])</f>
-        <v>0</v>
+        <v>5700</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -2785,310 +2731,320 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B22" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="C22" s="50"/>
+      <c r="D22" s="50">
+        <f>SUMIF('Account Balance'!B:B,OtherAssets[[#This Row],[Other assets:]],'Account Balance'!C:C)</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B23" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="24">
-        <v>0</v>
-      </c>
-      <c r="D22" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B23" s="26" t="s">
+      <c r="C23" s="24">
+        <v>0</v>
+      </c>
+      <c r="D23" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B24" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="C23" s="27">
+      <c r="C24" s="27">
         <f>SUBTOTAL(109,OtherAssets[Previous Year])</f>
         <v>0</v>
       </c>
-      <c r="D23" s="27">
+      <c r="D24" s="27">
         <f>SUBTOTAL(109,OtherAssets[Current Year])</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B24" s="28"/>
-      <c r="C24" s="29"/>
-      <c r="D24" s="30"/>
-    </row>
-    <row r="25" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="18" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B25" s="28"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="30"/>
+    </row>
+    <row r="26" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="B25" s="31" t="s">
+      <c r="B26" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="C25" s="32">
+      <c r="C26" s="32">
         <f>OtherAssets[[#Totals],[Previous Year]]+FixedAssets[[#Totals],[Previous Year]]+CurrentAssets[[#Totals],[Previous Year]]</f>
         <v>0</v>
       </c>
-      <c r="D25" s="32">
+      <c r="D26" s="32">
         <f>OtherAssets[[#Totals],[Current Year]]+FixedAssets[[#Totals],[Current Year]]+CurrentAssets[[#Totals],[Current Year]]</f>
-        <v>8300</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B26" s="33"/>
-      <c r="C26" s="34"/>
-      <c r="D26" s="34"/>
-    </row>
-    <row r="27" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="18" t="s">
+        <v>9100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B27" s="33"/>
+      <c r="C27" s="34"/>
+      <c r="D27" s="34"/>
+    </row>
+    <row r="28" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="B27" s="35" t="s">
+      <c r="B28" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="C27" s="36"/>
-      <c r="D27" s="37"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="18" t="s">
+      <c r="C28" s="36"/>
+      <c r="D28" s="37"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="B28" s="38" t="s">
+      <c r="B29" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="C28" s="39" t="s">
+      <c r="C29" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="D28" s="39" t="s">
+      <c r="D29" s="39" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B29" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="C29" s="41">
-        <v>0</v>
-      </c>
-      <c r="D29" s="41">
-        <f>SUMIF('Account Balance'!A:A,CurrentLiabilities[[#This Row],[Current liabilities:]],'Account Balance'!B:B)</f>
-        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B30" s="40" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C30" s="41">
         <v>0</v>
       </c>
       <c r="D30" s="41">
-        <f>SUMIF('Account Balance'!A:A,CurrentLiabilities[[#This Row],[Current liabilities:]],'Account Balance'!B:B)</f>
-        <v>0</v>
+        <f>SUMIF('Account Balance'!B:B,CurrentLiabilities[[#This Row],[Current liabilities:]],'Account Balance'!C:C)</f>
+        <v>800</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B31" s="40" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="C31" s="41">
         <v>0</v>
       </c>
       <c r="D31" s="41">
-        <f>SUMIF('Account Balance'!A:A,CurrentLiabilities[[#This Row],[Current liabilities:]],'Account Balance'!B:B)</f>
+        <f>SUMIF('Account Balance'!B:B,CurrentLiabilities[[#This Row],[Current liabilities:]],'Account Balance'!C:C)</f>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B32" s="40" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C32" s="41">
         <v>0</v>
       </c>
       <c r="D32" s="41">
-        <f>SUMIF('Account Balance'!A:A,CurrentLiabilities[[#This Row],[Current liabilities:]],'Account Balance'!B:B)</f>
+        <f>SUMIF('Account Balance'!B:B,CurrentLiabilities[[#This Row],[Current liabilities:]],'Account Balance'!C:C)</f>
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B33" s="40" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C33" s="41">
         <v>0</v>
       </c>
       <c r="D33" s="41">
-        <f>SUMIF('Account Balance'!A:A,CurrentLiabilities[[#This Row],[Current liabilities:]],'Account Balance'!B:B)</f>
+        <f>SUMIF('Account Balance'!B:B,CurrentLiabilities[[#This Row],[Current liabilities:]],'Account Balance'!C:C)</f>
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B34" s="40" t="s">
-        <v>63</v>
-      </c>
-      <c r="C34" s="41"/>
+        <v>9</v>
+      </c>
+      <c r="C34" s="41">
+        <v>0</v>
+      </c>
       <c r="D34" s="41">
-        <f>SUMIF('Account Balance'!A:A,CurrentLiabilities[[#This Row],[Current liabilities:]],'Account Balance'!B:B)</f>
-        <v>5100</v>
+        <f>SUMIF('Account Balance'!B:B,CurrentLiabilities[[#This Row],[Current liabilities:]],'Account Balance'!C:C)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B35" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="C35" s="41"/>
+      <c r="D35" s="41">
+        <f>SUMIF('Account Balance'!B:B,CurrentLiabilities[[#This Row],[Current liabilities:]],'Account Balance'!C:C)</f>
+        <v>5100</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B36" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="C35" s="41">
-        <v>0</v>
-      </c>
-      <c r="D35" s="41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B36" s="42" t="s">
+      <c r="C36" s="41">
+        <v>0</v>
+      </c>
+      <c r="D36" s="41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B37" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="C36" s="43">
+      <c r="C37" s="43">
         <f>SUBTOTAL(109,CurrentLiabilities[Previous Year])</f>
         <v>0</v>
       </c>
-      <c r="D36" s="43">
+      <c r="D37" s="43">
         <f>SUBTOTAL(109,CurrentLiabilities[Current Year])</f>
-        <v>5100</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B37" s="25"/>
-      <c r="C37" s="25"/>
-      <c r="D37" s="25"/>
+        <v>5900</v>
+      </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="18" t="s">
+      <c r="B38" s="25"/>
+      <c r="C38" s="25"/>
+      <c r="D38" s="25"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="B38" s="38" t="s">
+      <c r="B39" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="C38" s="39" t="s">
+      <c r="C39" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="D38" s="39" t="s">
+      <c r="D39" s="39" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B39" s="40" t="s">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B40" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="C39" s="41">
-        <v>0</v>
-      </c>
-      <c r="D39" s="41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B40" s="42" t="s">
+      <c r="C40" s="41">
+        <v>0</v>
+      </c>
+      <c r="D40" s="41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B41" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="C40" s="43">
+      <c r="C41" s="43">
         <f>SUBTOTAL(109,LongTermLiabilities[Previous Year])</f>
         <v>0</v>
       </c>
-      <c r="D40" s="43">
+      <c r="D41" s="43">
         <f>SUBTOTAL(109,LongTermLiabilities[Current Year])</f>
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B41" s="25"/>
-      <c r="C41" s="25"/>
-      <c r="D41" s="25"/>
-    </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="18" t="s">
+      <c r="B42" s="25"/>
+      <c r="C42" s="25"/>
+      <c r="D42" s="25"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="B42" s="38" t="s">
+      <c r="B43" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="C42" s="39" t="s">
+      <c r="C43" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="D42" s="39" t="s">
+      <c r="D43" s="39" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B43" s="40" t="s">
-        <v>61</v>
-      </c>
-      <c r="C43" s="41">
-        <v>0</v>
-      </c>
-      <c r="D43" s="41">
-        <f>SUMIF('Account Balance'!A:A,OwnersEquity[[#This Row],[Owner''s equity:]],'Account Balance'!B:B)</f>
-        <v>3200</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B44" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="C44" s="41">
+        <v>0</v>
+      </c>
+      <c r="D44" s="41">
+        <f>SUMIF('Account Balance'!B:B,OwnersEquity[[#This Row],[Owner''s equity:]],'Account Balance'!C:C)</f>
+        <v>3200</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B45" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="C44" s="41">
-        <v>0</v>
-      </c>
-      <c r="D44" s="41">
-        <f>SUMIF('Account Balance'!A:A,OwnersEquity[[#This Row],[Owner''s equity:]],'Account Balance'!B:B)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B45" s="42" t="s">
+      <c r="C45" s="41">
+        <v>0</v>
+      </c>
+      <c r="D45" s="41">
+        <f>SUMIF('Account Balance'!B:B,OwnersEquity[[#This Row],[Owner''s equity:]],'Account Balance'!C:C)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B46" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="C45" s="43">
+      <c r="C46" s="43">
         <f>SUBTOTAL(109,OwnersEquity[Previous Year])</f>
         <v>0</v>
       </c>
-      <c r="D45" s="43">
+      <c r="D46" s="43">
         <f>SUBTOTAL(109,OwnersEquity[Current Year])</f>
         <v>3200</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B46" s="6"/>
-      <c r="C46" s="7"/>
-      <c r="D46" s="8"/>
-    </row>
-    <row r="47" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="18" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B47" s="6"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="8"/>
+    </row>
+    <row r="48" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A48" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="B47" s="9" t="s">
+      <c r="B48" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C47" s="15">
+      <c r="C48" s="15">
         <f>OwnersEquity[[#Totals],[Previous Year]]+LongTermLiabilities[[#Totals],[Previous Year]]+CurrentLiabilities[[#Totals],[Previous Year]]</f>
         <v>0</v>
       </c>
-      <c r="D47" s="15">
+      <c r="D48" s="15">
         <f>OwnersEquity[[#Totals],[Current Year]]+LongTermLiabilities[[#Totals],[Current Year]]+CurrentLiabilities[[#Totals],[Current Year]]</f>
-        <v>8300</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="14.4" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="10"/>
-      <c r="C48" s="11"/>
-      <c r="D48" s="12"/>
-    </row>
-    <row r="50" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A50" s="18" t="s">
+        <v>9100</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="14.4" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B49" s="10"/>
+      <c r="C49" s="11"/>
+      <c r="D49" s="12"/>
+    </row>
+    <row r="51" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A51" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="B50" s="14" t="s">
+      <c r="B51" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C50" s="16">
-        <f>SUM(C25-C47)</f>
-        <v>0</v>
-      </c>
-      <c r="D50" s="16">
-        <f>SUM(D25-D47)</f>
+      <c r="C51" s="16">
+        <f>SUM(C26-C48)</f>
+        <v>0</v>
+      </c>
+      <c r="D51" s="16">
+        <f>SUM(D26-D48)</f>
         <v>0</v>
       </c>
     </row>
@@ -3098,8 +3054,8 @@
     <mergeCell ref="D1:D2"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
-  <conditionalFormatting sqref="C50:D50">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="lessThan">
+  <conditionalFormatting sqref="C51:D51">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3121,15 +3077,15 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A17E8F0C-18AE-4F1C-BFCB-6861AFF7E71B}">
   <sheetPr published="0"/>
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="84.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
@@ -3140,6 +3096,26 @@
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -3151,47 +3127,158 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E7A4FB2-9A50-4EE3-A1DC-2FD855DC911D}">
   <sheetPr published="0"/>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="48" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="B1">
+      <c r="C1">
         <v>3200</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="48" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>5100</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="49" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3">
+        <v>-5700</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="44" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>5700</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="44" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6">
+        <v>-150</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="44" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8">
+        <v>-1600</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9" s="44" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>6</v>
+      </c>
+      <c r="B10" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10">
+        <v>-1200</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="B3">
+      <c r="C11">
         <v>5100</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="49" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12" s="45" t="s">
         <v>61</v>
       </c>
-      <c r="B4">
+      <c r="C12">
         <v>3200</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>5</v>
+      </c>
+      <c r="B13" s="45" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13">
+        <v>800</v>
       </c>
     </row>
   </sheetData>

</xml_diff>